<commit_message>
Fix check for dimension level codes and text and clean up a bunch of stuff
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests7.xlsx
+++ b/tests/testthat/testdata/struct_tests7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA30FF81-DF75-4D31-A3A9-92B362C9D26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEBF02B-5EDB-4827-A60E-87CBF89721E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-1245" windowWidth="19440" windowHeight="15150" xr2:uid="{02901389-53B7-4262-B2DF-D4865029EACE}"/>
+    <workbookView xWindow="210" yWindow="150" windowWidth="25170" windowHeight="15300" xr2:uid="{02901389-53B7-4262-B2DF-D4865029EACE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>source</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>umar, eurostat</t>
-  </si>
-  <si>
-    <t>umar eurostat</t>
   </si>
 </sst>
 </file>
@@ -499,7 +496,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +576,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>

</xml_diff>